<commit_message>
About pages excel updated
</commit_message>
<xml_diff>
--- a/Final report/About Page/Testing Spreadsheet v1.0 AboutPage.xlsx
+++ b/Final report/About Page/Testing Spreadsheet v1.0 AboutPage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_Toc407532261" localSheetId="0">Reqs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="216">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -395,9 +395,6 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>Not execited</t>
-  </si>
-  <si>
     <t>Stats on Test case runs</t>
   </si>
   <si>
@@ -416,18 +413,6 @@
     <t>To show that when Order is selected as a logged in user on the About page, the user is directed to the Order page.</t>
   </si>
   <si>
-    <t>Nav_TCon_1</t>
-  </si>
-  <si>
-    <t>Nav_TCon_2</t>
-  </si>
-  <si>
-    <t>Nav_TCon_3</t>
-  </si>
-  <si>
-    <t>Nav_TCon_4</t>
-  </si>
-  <si>
     <t>4.1.20</t>
   </si>
   <si>
@@ -437,15 +422,6 @@
     <t>To show that when Order is selected as a non-logged in user on the About page, the user is prevented from accessing the Order page</t>
   </si>
   <si>
-    <t>Nav_TCon_5</t>
-  </si>
-  <si>
-    <t>Nav_TCon_6</t>
-  </si>
-  <si>
-    <t>Nav_TCon_7</t>
-  </si>
-  <si>
     <t>TCase_1</t>
   </si>
   <si>
@@ -641,9 +617,6 @@
     <t>4.1.4</t>
   </si>
   <si>
-    <t>low</t>
-  </si>
-  <si>
     <t>4.1.19</t>
   </si>
   <si>
@@ -683,24 +656,6 @@
     <t>Check if the About page contains textual information</t>
   </si>
   <si>
-    <t>Nav_TCon_8</t>
-  </si>
-  <si>
-    <t>Nav_TCon_9</t>
-  </si>
-  <si>
-    <t>Nav_TCon_10</t>
-  </si>
-  <si>
-    <t>Nav_TCon_11</t>
-  </si>
-  <si>
-    <t>Nav_TCon_12</t>
-  </si>
-  <si>
-    <t>Nav_TCon_13</t>
-  </si>
-  <si>
     <t>About_TProc_9</t>
   </si>
   <si>
@@ -767,12 +722,6 @@
     <t>Fine</t>
   </si>
   <si>
-    <t>About_1</t>
-  </si>
-  <si>
-    <t>About_2</t>
-  </si>
-  <si>
     <t>Opens in the same tab therefore leaving the Pizza website</t>
   </si>
   <si>
@@ -794,33 +743,18 @@
     <t>4.1.5</t>
   </si>
   <si>
-    <t>About_Tconn_14</t>
-  </si>
-  <si>
     <t>To show that the About page exists as part of the website system</t>
   </si>
   <si>
     <t>4.1.9</t>
   </si>
   <si>
-    <t>About_Tconn_15</t>
-  </si>
-  <si>
     <t>4.1.10</t>
   </si>
   <si>
     <t>4.1.11</t>
   </si>
   <si>
-    <t>About_Tconn_16</t>
-  </si>
-  <si>
-    <t>About_Tconn_17</t>
-  </si>
-  <si>
-    <t>About_Tconn_18</t>
-  </si>
-  <si>
     <t>To show that a non-logged in user can directly navigate to the "Register" and "Log in" pages from the "About" page</t>
   </si>
   <si>
@@ -836,9 +770,6 @@
     <t>Check if the About page exists as part of the website</t>
   </si>
   <si>
-    <t>Nav_TCon_14</t>
-  </si>
-  <si>
     <t>TCase_14</t>
   </si>
   <si>
@@ -881,18 +812,6 @@
     <t>Check if the Log in page can be directly navigated to from the About page as a non-logged in user</t>
   </si>
   <si>
-    <t>Nav_TCon_15</t>
-  </si>
-  <si>
-    <t>Nav_TCon_16</t>
-  </si>
-  <si>
-    <t>Nav_TCon_17</t>
-  </si>
-  <si>
-    <t>Nav_TCon_18</t>
-  </si>
-  <si>
     <t>User is directed to the Register page</t>
   </si>
   <si>
@@ -911,9 +830,6 @@
     <t>About_TProc_19</t>
   </si>
   <si>
-    <t>Nav_TCon_19</t>
-  </si>
-  <si>
     <t>Check if the My Account - reset password page can be directly navigated to from the About page as a logged in user</t>
   </si>
   <si>
@@ -939,6 +855,30 @@
   </si>
   <si>
     <t>While on the About page check if the Forgot password page is directly accessible</t>
+  </si>
+  <si>
+    <t>About_TConn_14</t>
+  </si>
+  <si>
+    <t>About_TConn_15</t>
+  </si>
+  <si>
+    <t>About_TConn_16</t>
+  </si>
+  <si>
+    <t>About_TConn_17</t>
+  </si>
+  <si>
+    <t>About_TConn_18</t>
+  </si>
+  <si>
+    <t>About_Defect_1</t>
+  </si>
+  <si>
+    <t>About_Defect_2</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1290,7 @@
                   <c:v>Failed</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Not execited</c:v>
+                  <c:v>Not executed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1485,11 +1425,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101920128"/>
-        <c:axId val="101926016"/>
+        <c:axId val="46083456"/>
+        <c:axId val="46089344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101920128"/>
+        <c:axId val="46083456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1439,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101926016"/>
+        <c:crossAx val="46089344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101926016"/>
+        <c:axId val="46089344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101920128"/>
+        <c:crossAx val="46083456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1927,8 +1867,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,16 +1894,16 @@
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>41</v>
@@ -1971,13 +1911,13 @@
     </row>
     <row r="3" spans="1:9" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -1986,13 +1926,13 @@
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -2003,16 +1943,16 @@
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>43</v>
@@ -2020,13 +1960,13 @@
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -2037,13 +1977,13 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -2054,13 +1994,13 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -2071,13 +2011,13 @@
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -2085,13 +2025,13 @@
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -2099,13 +2039,13 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -2113,41 +2053,41 @@
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -2155,13 +2095,13 @@
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -2169,13 +2109,13 @@
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -2183,13 +2123,13 @@
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -2197,13 +2137,13 @@
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -2211,13 +2151,13 @@
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -2248,9 +2188,7 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AE27" sqref="AE27"/>
-    </sheetView>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2263,7 +2201,7 @@
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
@@ -2322,22 +2260,22 @@
     </row>
     <row r="2" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G2" s="31">
         <v>42080</v>
@@ -2346,7 +2284,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -2361,19 +2299,19 @@
     </row>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -2385,7 +2323,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
@@ -2400,19 +2338,19 @@
     </row>
     <row r="4" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>6</v>
@@ -2424,7 +2362,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="4"/>
@@ -2439,22 +2377,22 @@
     </row>
     <row r="5" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G5" s="31">
         <v>42080</v>
@@ -2463,7 +2401,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="4"/>
@@ -2475,19 +2413,19 @@
     </row>
     <row r="6" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
@@ -2499,7 +2437,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="4"/>
@@ -2511,19 +2449,19 @@
     </row>
     <row r="7" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -2535,7 +2473,7 @@
         <v>24</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="4"/>
@@ -2545,24 +2483,24 @@
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
       <c r="T7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -2574,7 +2512,7 @@
         <v>24</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="4"/>
@@ -2593,19 +2531,19 @@
     </row>
     <row r="9" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
@@ -2617,10 +2555,10 @@
         <v>25</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>33</v>
@@ -2633,7 +2571,7 @@
       </c>
       <c r="N9" s="31"/>
       <c r="O9" s="10" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="P9" s="10"/>
       <c r="T9" t="s">
@@ -2646,19 +2584,19 @@
     </row>
     <row r="10" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
@@ -2670,7 +2608,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="4"/>
@@ -2680,7 +2618,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="T10" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="U10" s="30">
         <f>COUNTIF(H2:H90,"*Not*")</f>
@@ -2689,19 +2627,19 @@
     </row>
     <row r="11" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
@@ -2713,7 +2651,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="4"/>
@@ -2725,19 +2663,19 @@
     </row>
     <row r="12" spans="1:26" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -2749,10 +2687,10 @@
         <v>25</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>33</v>
@@ -2765,25 +2703,25 @@
       </c>
       <c r="N12" s="31"/>
       <c r="O12" s="10" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>27</v>
@@ -2795,7 +2733,7 @@
         <v>24</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -2807,19 +2745,19 @@
     </row>
     <row r="14" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>11</v>
@@ -2831,7 +2769,7 @@
         <v>24</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -2843,21 +2781,23 @@
     </row>
     <row r="15" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F15" s="11"/>
+        <v>208</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G15" s="31">
         <v>42108</v>
       </c>
@@ -2865,7 +2805,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -2877,21 +2817,23 @@
     </row>
     <row r="16" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F16" s="11"/>
+        <v>209</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="G16" s="31">
         <v>42108</v>
       </c>
@@ -2899,7 +2841,7 @@
         <v>24</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -2911,21 +2853,23 @@
     </row>
     <row r="17" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F17" s="11"/>
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G17" s="31">
         <v>42108</v>
       </c>
@@ -2933,7 +2877,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -2945,21 +2889,23 @@
     </row>
     <row r="18" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="F18" s="11"/>
+      <c r="F18" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G18" s="31">
         <v>42108</v>
       </c>
@@ -2967,7 +2913,7 @@
         <v>24</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -2979,21 +2925,23 @@
     </row>
     <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G19" s="31">
         <v>42108</v>
       </c>
@@ -3001,7 +2949,7 @@
         <v>24</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -3013,21 +2961,23 @@
     </row>
     <row r="20" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F20" s="11"/>
+        <v>212</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G20" s="31">
         <v>42108</v>
       </c>
@@ -3035,7 +2985,7 @@
         <v>24</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -3115,7 +3065,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="T25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3153,7 +3103,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="T27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U27" s="30">
         <f>COUNTIF(L2:L50,"*Moderate*")</f>
@@ -5067,6 +5017,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Settings!$B$4:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5077,8 +5039,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5120,19 +5082,19 @@
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="26" t="s">
@@ -5146,19 +5108,19 @@
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -5171,19 +5133,19 @@
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -5196,19 +5158,19 @@
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -5221,19 +5183,19 @@
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -5246,19 +5208,19 @@
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -5271,19 +5233,19 @@
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -5296,19 +5258,19 @@
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -5321,19 +5283,19 @@
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -5346,19 +5308,19 @@
     </row>
     <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -5371,19 +5333,19 @@
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -5396,19 +5358,19 @@
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -5421,19 +5383,19 @@
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -5446,19 +5408,19 @@
     </row>
     <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -5471,19 +5433,19 @@
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -5496,19 +5458,19 @@
     </row>
     <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -5521,19 +5483,19 @@
     </row>
     <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -5546,19 +5508,19 @@
     </row>
     <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -5571,19 +5533,19 @@
     </row>
     <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -5646,7 +5608,7 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -5679,6 +5641,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5792,32 +5769,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -5832,9 +5787,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>